<commit_message>
Updated with attachment extraction
</commit_message>
<xml_diff>
--- a/OpenRequests.xlsx
+++ b/OpenRequests.xlsx
@@ -8,14 +8,14 @@
     <sheet name="Requests" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Requests'!$A$1:$L$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Requests'!$A$1:$L$16</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>RequestID</t>
   </si>
@@ -224,6 +224,15 @@
     <t>SOW-745</t>
   </si>
   <si>
+    <t>SOW-753 - Clark Hill PLC - Time Upgrade to Support Outlook 365</t>
+  </si>
+  <si>
+    <t>SOW-753</t>
+  </si>
+  <si>
+    <t>10,000</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOW-754 - Sidley Austin LLP - Walls/AT Upgrade </t>
   </si>
   <si>
@@ -252,6 +261,18 @@
   </si>
   <si>
     <t>65,000</t>
+  </si>
+  <si>
+    <t>SOW-768 - Ogletree, Deakins, Nash, Smoak &amp; Stewart, P.C. - Ogletree Deakins - Open Phase 2 - Bill Groups and Rates</t>
+  </si>
+  <si>
+    <t>SOW-768</t>
+  </si>
+  <si>
+    <t>Open - Intake</t>
+  </si>
+  <si>
+    <t>11,250</t>
   </si>
 </sst>
 </file>
@@ -297,7 +318,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -723,7 +744,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>69</v>
@@ -738,10 +759,10 @@
         <v>15</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>70</v>
@@ -750,21 +771,21 @@
         <v>33</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>13</v>
@@ -776,67 +797,143 @@
         <v>15</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="K13" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
+        <v>177</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
         <v>179</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="B15" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G15" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="0" t="s">
+      <c r="H15" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>78</v>
+      <c r="J15" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>201</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L14"/>
+  <autoFilter ref="A1:L16"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Attachments, Grid answer, config changes
</commit_message>
<xml_diff>
--- a/OpenRequests.xlsx
+++ b/OpenRequests.xlsx
@@ -8,14 +8,14 @@
     <sheet name="Requests" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Requests'!$A$1:$L$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Requests'!$A$1:$L$18</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>RequestID</t>
   </si>
@@ -59,7 +59,8 @@
     <t>Fixed Fee</t>
   </si>
   <si>
-    <t>&lt;Invalid question type&gt;</t>
+    <t xml:space="preserve">2019-08-02T00:00:00Z|Praj Kulkarni|Create formal SOW and send to Steve Spera. |true|
+</t>
   </si>
   <si>
     <t>250</t>
@@ -89,6 +90,11 @@
     <t>SOW-694 - McGuire Woods - Intapp Walls - Add Legal Holds</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-08-02T00:00:00Z|Praj Kulkarni|Create SOW and send it to client.|true|
+2019-08-05T00:00:00Z|Praj Kulkarni|Update SOW based on their feedback and resend|2019-08-06T00:00:00Z|false|
+</t>
+  </si>
+  <si>
     <t>SOW-694</t>
   </si>
   <si>
@@ -104,6 +110,10 @@
     <t>Time &amp; Materials Estimate</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-08-14T00:00:00Z|Max Garcia|send out SOW|2019-08-13T00:00:00Z|true|
+</t>
+  </si>
+  <si>
     <t>275</t>
   </si>
   <si>
@@ -131,6 +141,10 @@
     <t>SOW-704 - Fenwick &amp; West LLP - iManage Cloud Consulting</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-08-13T00:00:00Z|Praj Kulkarni|Follow up with them if they haven't responded.|2019-08-24T00:00:00Z|false|
+</t>
+  </si>
+  <si>
     <t>SOW-704</t>
   </si>
   <si>
@@ -143,6 +157,10 @@
     <t>SOW-711 - Richards, Layton &amp; Finger, P.A. - Intapp Flow - Check Request CID</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-08-19T00:00:00Z|Jeff Armbrecht|Send SOW|2019-08-23T00:00:00Z|true|
+</t>
+  </si>
+  <si>
     <t>Flow</t>
   </si>
   <si>
@@ -161,6 +179,10 @@
     <t xml:space="preserve">SOW-730 - Glaser, Weil, Fink, Jacobs, Howard, Avchen &amp; Shapiro, LLP - Intapp Time &amp; Mobile </t>
   </si>
   <si>
+    <t xml:space="preserve">2019-09-27T00:00:00Z|Bob Fishel|Follow up with Cora on meeting and update Lori |false|
+</t>
+  </si>
+  <si>
     <t>Time</t>
   </si>
   <si>
@@ -182,6 +204,10 @@
     <t>SOW-733 - Arnall Golden Gregory LLP - Intapp Flow/Integrate Training</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-09-27T00:00:00Z|Alastair Seddon|Create Draft SOW and distribute to Jeff and Alan.|2019-09-27T00:00:00Z|false|
+</t>
+  </si>
+  <si>
     <t>Integrate</t>
   </si>
   <si>
@@ -200,6 +226,10 @@
     <t xml:space="preserve">SOW-740 - Kilpatrick Townsend &amp; Stockton LLP - On-Going Support </t>
   </si>
   <si>
+    <t xml:space="preserve">2019-10-23T00:00:00Z|Suzi Hellwege|Follow-up on completed contract |false|
+</t>
+  </si>
+  <si>
     <t>SOW-740</t>
   </si>
   <si>
@@ -209,6 +239,10 @@
     <t xml:space="preserve">SOW-743 - Fenwick &amp; West LLP - Walls Upgrade </t>
   </si>
   <si>
+    <t xml:space="preserve">2019-10-26T00:00:00Z|Praj Kulkarni|Follow-up with Helen on signed contract |false|
+</t>
+  </si>
+  <si>
     <t>Praj Kulkarni</t>
   </si>
   <si>
@@ -221,12 +255,20 @@
     <t xml:space="preserve">SOW-745 - Goodwin Procter LLP - Walls On-Going Support </t>
   </si>
   <si>
+    <t xml:space="preserve">2019-11-01T00:00:00Z|Suzi Hellwege|Follow-up on SOW with firm |false|
+</t>
+  </si>
+  <si>
     <t>SOW-745</t>
   </si>
   <si>
     <t>SOW-753 - Clark Hill PLC - Time Upgrade to Support Outlook 365</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-11-06T00:00:00Z|Bob Fishel|Meet with firm to discuss upgrade options|false|
+</t>
+  </si>
+  <si>
     <t>SOW-753</t>
   </si>
   <si>
@@ -236,12 +278,20 @@
     <t xml:space="preserve">SOW-754 - Sidley Austin LLP - Walls/AT Upgrade </t>
   </si>
   <si>
+    <t xml:space="preserve">2019-11-09T00:00:00Z|Praj Kulkarni|Follow-up with Tim Nolan @ Intapp on this opportunity |false|
+</t>
+  </si>
+  <si>
     <t>SOW-754</t>
   </si>
   <si>
     <t>SOW-757 - Vorys, Sater, Seymour and Pease LLP - Vorys - Support Hours</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-11-15T00:00:00Z|Alastair Seddon|Finish SOW.|2019-11-15T00:00:00Z|false|
+</t>
+  </si>
+  <si>
     <t>SOW-757</t>
   </si>
   <si>
@@ -254,6 +304,10 @@
     <t xml:space="preserve">SOW-756 - Ropers Majeski Kohn &amp; Bentley - Intapp Total Time On Prem </t>
   </si>
   <si>
+    <t xml:space="preserve">2019-11-21T00:00:00Z|Bob Fishel|Follow up with firm |false|
+</t>
+  </si>
+  <si>
     <t>SOW-756</t>
   </si>
   <si>
@@ -263,9 +317,29 @@
     <t>65,000</t>
   </si>
   <si>
+    <t xml:space="preserve">SOW-761 - Davis Polk &amp; Wardwell LLP - Insiders Module </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-11-23T00:00:00Z|Suzi Hellwege|Follow-up on SOW with Janet |false|
+</t>
+  </si>
+  <si>
+    <t>SOW-761</t>
+  </si>
+  <si>
+    <t>New Module/Extension</t>
+  </si>
+  <si>
+    <t>7,500</t>
+  </si>
+  <si>
     <t>SOW-768 - Ogletree, Deakins, Nash, Smoak &amp; Stewart, P.C. - Ogletree Deakins - Open Phase 2 - Bill Groups and Rates</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-11-21T00:00:00Z|Alastair Seddon|Prepare SOW|2019-11-21T00:00:00Z|false|
+</t>
+  </si>
+  <si>
     <t>SOW-768</t>
   </si>
   <si>
@@ -273,6 +347,20 @@
   </si>
   <si>
     <t>11,250</t>
+  </si>
+  <si>
+    <t>SOW-771 - Holland &amp; Knight - Upgrade Open to Latest Version (5.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-11-27T00:00:00Z|Max Garcia|max to send SOW after receiving information from HK about APIs in use.|2019-12-11T00:00:00Z|true|
+2019-12-05T00:00:00Z|Max Garcia|Send SOW|2019-12-05T00:00:00Z|true|
+</t>
+  </si>
+  <si>
+    <t>SOW-771</t>
+  </si>
+  <si>
+    <t>Upgrade, Training, Open - Intake, Open - Conflicts</t>
   </si>
 </sst>
 </file>
@@ -318,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -411,7 +499,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>15</v>
@@ -423,19 +511,19 @@
         <v>17</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -443,37 +531,37 @@
         <v>112</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -481,13 +569,13 @@
         <v>116</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>15</v>
@@ -499,19 +587,19 @@
         <v>17</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -519,37 +607,37 @@
         <v>122</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -557,37 +645,37 @@
         <v>148</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
@@ -595,37 +683,37 @@
         <v>151</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
@@ -633,13 +721,13 @@
         <v>160</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>15</v>
@@ -651,19 +739,19 @@
         <v>17</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K9" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10">
@@ -671,13 +759,13 @@
         <v>164</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>15</v>
@@ -686,10 +774,10 @@
         <v>16</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>19</v>
@@ -701,7 +789,7 @@
         <v>21</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
@@ -709,13 +797,13 @@
         <v>166</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>15</v>
@@ -724,22 +812,22 @@
         <v>16</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12">
@@ -747,37 +835,37 @@
         <v>171</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13">
@@ -785,13 +873,13 @@
         <v>173</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>15</v>
@@ -800,13 +888,13 @@
         <v>16</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>20</v>
@@ -815,7 +903,7 @@
         <v>21</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
@@ -823,37 +911,37 @@
         <v>177</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="K14" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15">
@@ -861,79 +949,155 @@
         <v>179</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="K15" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="K16" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>85</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>201</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>206</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L16"/>
+  <autoFilter ref="A1:L18"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>